<commit_message>
update redundant vehicle/route handling
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D70687-2DEF-49AA-A485-06189671825D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD116287-063D-4AA5-9503-C9BAB3093935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,7 +788,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1718,15 +1718,15 @@
         <v>1.5463919864454168E-2</v>
       </c>
       <c r="F65" s="5">
-        <f>4.89/1000</f>
-        <v>4.8899999999999994E-3</v>
+        <f>4.75/1000</f>
+        <v>4.7499999999999999E-3</v>
       </c>
       <c r="G65" s="1">
         <v>2000</v>
       </c>
       <c r="H65" s="6">
         <f>F65 * G65</f>
-        <v>9.7799999999999994</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -1747,15 +1747,15 @@
         <v>-2.2251890941430874E-2</v>
       </c>
       <c r="F66" s="4">
-        <f>14.59/1000</f>
-        <v>1.4590000000000001E-2</v>
+        <f>14.52/1000</f>
+        <v>1.452E-2</v>
       </c>
       <c r="G66" s="1">
         <v>2000</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ref="H66:H70" si="1">F66 * G66</f>
-        <v>29.18</v>
+        <v>29.04</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -1776,15 +1776,15 @@
         <v>-3.7795946908891764E-6</v>
       </c>
       <c r="F67" s="4">
-        <f>6.21/1000</f>
-        <v>6.2100000000000002E-3</v>
+        <f>6.25/1000</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="G67" s="1">
         <v>2000</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="1"/>
-        <v>12.42</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -1805,15 +1805,15 @@
         <v>-5.8207653255148983E-6</v>
       </c>
       <c r="F68" s="4">
-        <f>24.9/1000</f>
-        <v>2.4899999999999999E-2</v>
+        <f>25.3/1000</f>
+        <v>2.53E-2</v>
       </c>
       <c r="G68" s="1">
         <v>2000</v>
       </c>
       <c r="H68" s="6">
         <f t="shared" si="1"/>
-        <v>49.8</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -1834,15 +1834,15 @@
         <v>-1.6824405592926084E-2</v>
       </c>
       <c r="F69" s="4">
-        <f>5.11/1000</f>
-        <v>5.11E-3</v>
+        <f>4.99/1000</f>
+        <v>4.9900000000000005E-3</v>
       </c>
       <c r="G69" s="1">
         <v>2000</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" si="1"/>
-        <v>10.220000000000001</v>
+        <v>9.98</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -1863,15 +1863,15 @@
         <v>-3.7289699929135556E-2</v>
       </c>
       <c r="F70" s="4">
-        <f>15.56/1000</f>
-        <v>1.5560000000000001E-2</v>
+        <f>15.4/1000</f>
+        <v>1.54E-2</v>
       </c>
       <c r="G70" s="1">
         <v>2000</v>
       </c>
       <c r="H70" s="6">
         <f t="shared" si="1"/>
-        <v>31.12</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
limit vehicle routes, depot reopen, node removal
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F5C4BF-2355-4A8A-BE4A-47071AC79345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459A97F0-C598-492A-998B-EC1CC48AC8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="48309" windowHeight="26546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VRPTW Benchmarking" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="LRP Benchmarking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -321,11 +321,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000%"/>
-    <numFmt numFmtId="180" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -595,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -638,12 +637,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -657,8 +650,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,7 +941,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="A1:XFD1048576"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -1866,22 +1864,22 @@
         <v>1645.79</v>
       </c>
       <c r="D65" s="6">
-        <v>1647.99912450019</v>
+        <v>1660.6602148245399</v>
       </c>
       <c r="E65" s="3">
         <f>D65/C65-1</f>
-        <v>1.34228820213389E-3</v>
+        <v>9.0353051267415552E-3</v>
       </c>
       <c r="F65" s="5">
-        <f>4.5/1000</f>
-        <v>4.4999999999999997E-3</v>
+        <f>4.43/1000</f>
+        <v>4.4299999999999999E-3</v>
       </c>
       <c r="G65" s="1">
         <v>2000</v>
       </c>
       <c r="H65" s="6">
         <f>F65 * G65</f>
-        <v>9</v>
+        <v>8.86</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -1895,22 +1893,22 @@
         <v>1252.3699999999999</v>
       </c>
       <c r="D66" s="24">
-        <v>1201.06719688372</v>
+        <v>1198.8469022290501</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" ref="E66:E70" si="0">D66/C66-1</f>
-        <v>-4.0964573661361969E-2</v>
+        <v>-4.2737448015322754E-2</v>
       </c>
       <c r="F66" s="4">
-        <f>13.15/1000</f>
-        <v>1.315E-2</v>
+        <f>10.95/1000</f>
+        <v>1.095E-2</v>
       </c>
       <c r="G66" s="1">
         <v>2000</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ref="H66:H70" si="1">F66 * G66</f>
-        <v>26.3</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -1924,22 +1922,22 @@
         <v>828.94</v>
       </c>
       <c r="D67" s="6">
-        <v>828.93686694239898</v>
+        <v>828.93686694217695</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" si="0"/>
-        <v>-3.7795951468577726E-6</v>
+        <v>-3.7795954147545885E-6</v>
       </c>
       <c r="F67" s="4">
-        <f>6.39/1000</f>
-        <v>6.3899999999999998E-3</v>
+        <f>6.13/1000</f>
+        <v>6.13E-3</v>
       </c>
       <c r="G67" s="1">
         <v>2000</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="1"/>
-        <v>12.78</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -1953,22 +1951,22 @@
         <v>591.55999999999995</v>
       </c>
       <c r="D68" s="6">
-        <v>591.55655667036103</v>
+        <v>591.55655666910604</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="0"/>
-        <v>-5.8207614425098697E-6</v>
+        <v>-5.8207635639240252E-6</v>
       </c>
       <c r="F68" s="4">
-        <f>24.3/1000</f>
-        <v>2.4300000000000002E-2</v>
+        <f>19.07/1000</f>
+        <v>1.907E-2</v>
       </c>
       <c r="G68" s="1">
         <v>2000</v>
       </c>
       <c r="H68" s="6">
         <f t="shared" si="1"/>
-        <v>48.6</v>
+        <v>38.14</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -1982,22 +1980,22 @@
         <v>1696.94</v>
       </c>
       <c r="D69" s="6">
-        <v>1678.1751810066401</v>
+        <v>1664.75372917754</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="0"/>
-        <v>-1.1058033279526702E-2</v>
+        <v>-1.8967241518533351E-2</v>
       </c>
       <c r="F69" s="4">
-        <f>4.83/1000</f>
-        <v>4.8300000000000001E-3</v>
+        <f>4.77/1000</f>
+        <v>4.7699999999999999E-3</v>
       </c>
       <c r="G69" s="1">
         <v>2000</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" si="1"/>
-        <v>9.66</v>
+        <v>9.5399999999999991</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2011,22 +2009,22 @@
         <v>1406.91</v>
       </c>
       <c r="D70" s="24">
-        <v>1409.21629394568</v>
+        <v>1284.32614778683</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="0"/>
-        <v>1.6392618900142875E-3</v>
+        <v>-8.7129846410339051E-2</v>
       </c>
       <c r="F70" s="4">
-        <f>15.15/1000</f>
-        <v>1.515E-2</v>
+        <f>9.17/1000</f>
+        <v>9.1699999999999993E-3</v>
       </c>
       <c r="G70" s="1">
         <v>2000</v>
       </c>
       <c r="H70" s="6">
         <f t="shared" si="1"/>
-        <v>30.3</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2669,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5551421D-4FE7-47B7-A546-15E7A05240A9}">
   <dimension ref="A1:X280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -3841,16 +3839,16 @@
       <c r="B67" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27" t="s">
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
       <c r="I67" s="18" t="s">
         <v>3</v>
       </c>
@@ -3880,10 +3878,10 @@
       <c r="D68" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E68" s="31" t="s">
+      <c r="E68" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="F68" s="28" t="s">
+      <c r="F68" s="26" t="s">
         <v>86</v>
       </c>
       <c r="G68" s="25" t="s">
@@ -3907,38 +3905,38 @@
         <v>88</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="34">
+      <c r="C69" s="32">
         <v>3</v>
       </c>
-      <c r="D69" s="34">
+      <c r="D69" s="32">
         <v>5</v>
       </c>
-      <c r="E69" s="32">
+      <c r="E69" s="30">
         <v>54793</v>
       </c>
-      <c r="F69" s="34">
+      <c r="F69" s="32">
         <v>3</v>
       </c>
-      <c r="G69" s="34">
+      <c r="G69" s="32">
         <v>5</v>
       </c>
-      <c r="H69" s="29">
-        <v>55447.240290744303</v>
-      </c>
-      <c r="I69" s="37">
+      <c r="H69" s="27">
+        <v>55007.766132012403</v>
+      </c>
+      <c r="I69" s="34">
         <f>H69/E69-1</f>
-        <v>1.1940216647095436E-2</v>
+        <v>3.9195906778677347E-3</v>
       </c>
       <c r="J69" s="1">
-        <f>0.54/1000</f>
-        <v>5.4000000000000001E-4</v>
+        <f>0.38/1000</f>
+        <v>3.8000000000000002E-4</v>
       </c>
       <c r="K69" s="1">
-        <v>200</v>
-      </c>
-      <c r="L69" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L69" s="24">
         <f>K69*J69</f>
-        <v>0.108</v>
+        <v>0.76</v>
       </c>
       <c r="M69" s="12"/>
       <c r="N69" s="12"/>
@@ -3954,38 +3952,38 @@
         <v>89</v>
       </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="35">
+      <c r="C70" s="33">
         <v>2</v>
       </c>
-      <c r="D70" s="35">
+      <c r="D70" s="33">
         <v>6</v>
       </c>
-      <c r="E70" s="32">
+      <c r="E70" s="30">
         <v>63242</v>
       </c>
-      <c r="F70" s="35">
-        <v>3</v>
-      </c>
-      <c r="G70" s="35">
+      <c r="F70" s="33">
+        <v>2</v>
+      </c>
+      <c r="G70" s="33">
         <v>6</v>
       </c>
-      <c r="H70" s="30">
-        <v>70435.571795120006</v>
-      </c>
-      <c r="I70" s="36">
+      <c r="H70" s="28">
+        <v>68476.530907053006</v>
+      </c>
+      <c r="I70" s="34">
         <f>H70/E70-1</f>
-        <v>0.11374674733752888</v>
+        <v>8.2769850843632531E-2</v>
       </c>
       <c r="J70" s="1">
-        <f>3.72/1000</f>
-        <v>3.7200000000000002E-3</v>
+        <f>2.34/1000</f>
+        <v>2.3400000000000001E-3</v>
       </c>
       <c r="K70" s="1">
-        <v>200</v>
-      </c>
-      <c r="L70" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L70" s="24">
         <f>K70*J70</f>
-        <v>0.74399999999999999</v>
+        <v>4.68</v>
       </c>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -4001,39 +3999,39 @@
         <v>90</v>
       </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="35">
+      <c r="C71" s="33">
         <v>2</v>
       </c>
-      <c r="D71" s="35">
+      <c r="D71" s="33">
         <v>24</v>
       </c>
-      <c r="E71" s="32">
-        <v>199520</v>
-      </c>
-      <c r="F71" s="35">
-        <v>3</v>
-      </c>
-      <c r="G71" s="35">
+      <c r="E71" s="30">
+        <v>195568</v>
+      </c>
+      <c r="F71" s="33">
+        <v>2</v>
+      </c>
+      <c r="G71" s="33">
         <v>24</v>
       </c>
-      <c r="H71" s="30">
-        <v>249859.509590136</v>
-      </c>
-      <c r="I71" s="36">
+      <c r="H71" s="28">
+        <v>213864.368335242</v>
+      </c>
+      <c r="I71" s="34">
         <f>H71/E71-1</f>
-        <v>0.25230307533147567</v>
+        <v>9.3555020940245814E-2</v>
       </c>
       <c r="J71" s="1">
-        <f>7.96/1000</f>
-        <v>7.9600000000000001E-3</v>
+        <f>7.67/1000</f>
+        <v>7.6699999999999997E-3</v>
       </c>
       <c r="K71" s="1">
         <f>200 * 10</f>
         <v>2000</v>
       </c>
-      <c r="L71" s="1">
+      <c r="L71" s="24">
         <f>K71*J71</f>
-        <v>15.92</v>
+        <v>15.34</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
@@ -4041,39 +4039,39 @@
         <v>92</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="35">
+      <c r="C72" s="33">
         <v>3</v>
       </c>
-      <c r="D72" s="35">
+      <c r="D72" s="33">
         <v>11</v>
       </c>
-      <c r="E72" s="32">
+      <c r="E72" s="30">
         <v>204335</v>
       </c>
-      <c r="F72" s="35">
-        <v>4</v>
-      </c>
-      <c r="G72" s="35">
-        <v>8</v>
-      </c>
-      <c r="H72" s="30">
-        <v>270362.06230151601</v>
-      </c>
-      <c r="I72" s="36">
+      <c r="F72" s="33">
+        <v>3</v>
+      </c>
+      <c r="G72" s="33">
+        <v>11</v>
+      </c>
+      <c r="H72" s="28">
+        <v>216910.48921065999</v>
+      </c>
+      <c r="I72" s="34">
         <f t="shared" ref="I72:I73" si="0">H72/E72-1</f>
-        <v>0.32313143759765106</v>
-      </c>
-      <c r="J72" s="1">
-        <f>21.96/1000</f>
-        <v>2.196E-2</v>
+        <v>6.1543490888296137E-2</v>
+      </c>
+      <c r="J72" s="35">
+        <f>12.86/1000</f>
+        <v>1.286E-2</v>
       </c>
       <c r="K72" s="1">
         <f>200 * 10</f>
         <v>2000</v>
       </c>
-      <c r="L72" s="1">
+      <c r="L72" s="24">
         <f t="shared" ref="L72:L73" si="1">K72*J72</f>
-        <v>43.92</v>
+        <v>25.72</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
@@ -4081,38 +4079,38 @@
         <v>91</v>
       </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="34">
+      <c r="C73" s="32">
         <v>3</v>
       </c>
-      <c r="D73" s="34">
+      <c r="D73" s="32">
         <v>47</v>
       </c>
-      <c r="E73" s="33">
+      <c r="E73" s="31">
         <v>476684</v>
       </c>
-      <c r="F73" s="34">
+      <c r="F73" s="32">
         <v>4</v>
       </c>
-      <c r="G73" s="34">
-        <v>32</v>
-      </c>
-      <c r="H73" s="29">
-        <v>636757.505290751</v>
-      </c>
-      <c r="I73" s="36">
+      <c r="G73" s="32">
+        <v>47</v>
+      </c>
+      <c r="H73" s="27">
+        <v>614386.43483290798</v>
+      </c>
+      <c r="I73" s="34">
         <f t="shared" si="0"/>
-        <v>0.33580633142868432</v>
-      </c>
-      <c r="J73" s="38">
-        <f>50.9/1000</f>
-        <v>5.0900000000000001E-2</v>
+        <v>0.28887572235046277</v>
+      </c>
+      <c r="J73" s="35">
+        <f>42.97/1000</f>
+        <v>4.2970000000000001E-2</v>
       </c>
       <c r="K73" s="1">
         <v>3000</v>
       </c>
-      <c r="L73" s="1">
+      <c r="L73" s="24">
         <f t="shared" si="1"/>
-        <v>152.69999999999999</v>
+        <v>128.91</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
faster evaluation for non- time-window instances
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3438B00C-2328-4674-8E0E-F82579E04997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299F229D-E882-4A5F-B86B-BF7E07CC7F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="48309" windowHeight="26546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
   <si>
     <t>Best known</t>
   </si>
@@ -272,9 +272,6 @@
     <t>x = length(N)</t>
   </si>
   <si>
-    <t>n = ceil(x, digits=-(length(digits(x))-1))</t>
-  </si>
-  <si>
     <t>Vehicle Routing Problem with Time-Windows (VRPTW) Benchmarking</t>
   </si>
   <si>
@@ -315,6 +312,12 @@
   </si>
   <si>
     <t>coord100-10-2b</t>
+  </si>
+  <si>
+    <t>n = max(200, ceil(x, digits=-(length(digits(x))-1)))</t>
+  </si>
+  <si>
+    <t>n = max(500, ceil(x, digits=-(length(digits(x))-1)))</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -959,7 +962,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.05" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -1123,7 +1126,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -2668,7 +2671,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -2690,7 +2693,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.05" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -2894,7 +2897,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -3092,7 +3095,7 @@
     </row>
     <row r="30" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -3176,7 +3179,7 @@
     </row>
     <row r="34" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -3239,7 +3242,7 @@
     </row>
     <row r="37" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -3260,7 +3263,7 @@
     </row>
     <row r="38" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -3873,22 +3876,22 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="D68" s="25" t="s">
+      <c r="F68" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="F68" s="26" t="s">
+      <c r="G68" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H68" s="25" t="s">
         <v>86</v>
-      </c>
-      <c r="G68" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H68" s="25" t="s">
-        <v>87</v>
       </c>
       <c r="L68" s="12"/>
       <c r="M68" s="12"/>
@@ -3902,7 +3905,7 @@
     </row>
     <row r="69" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="32">
@@ -3921,22 +3924,22 @@
         <v>5</v>
       </c>
       <c r="H69" s="27">
-        <v>55873.872100158202</v>
+        <v>55449.609618147799</v>
       </c>
       <c r="I69" s="34">
         <f>H69/E69-1</f>
-        <v>1.9726463237242031E-2</v>
+        <v>1.1983458072158726E-2</v>
       </c>
       <c r="J69" s="1">
-        <f>0.41/1000</f>
-        <v>4.0999999999999999E-4</v>
+        <f>0.36/1000</f>
+        <v>3.5999999999999997E-4</v>
       </c>
       <c r="K69" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="L69" s="24">
         <f>K69*J69</f>
-        <v>0.82</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="M69" s="12"/>
       <c r="N69" s="12"/>
@@ -3949,7 +3952,7 @@
     </row>
     <row r="70" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="33">
@@ -3968,22 +3971,22 @@
         <v>6</v>
       </c>
       <c r="H70" s="28">
-        <v>69830.631383596206</v>
+        <v>64516.734565587001</v>
       </c>
       <c r="I70" s="34">
         <f>H70/E70-1</f>
-        <v>0.10418126219278645</v>
+        <v>2.0156455608409063E-2</v>
       </c>
       <c r="J70" s="35">
-        <f>2.5/1000</f>
-        <v>2.5000000000000001E-3</v>
+        <f>1.5/1000</f>
+        <v>1.5E-3</v>
       </c>
       <c r="K70" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="L70" s="24">
         <f>K70*J70</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -3996,7 +3999,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="33">
@@ -4012,18 +4015,18 @@
         <v>2</v>
       </c>
       <c r="G71" s="33">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H71" s="28">
-        <v>220723.237851224</v>
+        <v>207301.86896955999</v>
       </c>
       <c r="I71" s="34">
         <f>H71/E71-1</f>
-        <v>0.12862655368579734</v>
+        <v>5.9998920935735889E-2</v>
       </c>
       <c r="J71" s="1">
-        <f>8/1000</f>
-        <v>8.0000000000000002E-3</v>
+        <f>5.86/1000</f>
+        <v>5.8600000000000006E-3</v>
       </c>
       <c r="K71" s="1">
         <f>200 * 10</f>
@@ -4031,12 +4034,12 @@
       </c>
       <c r="L71" s="24">
         <f>K71*J71</f>
-        <v>16</v>
+        <v>11.72</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="33">
@@ -4055,28 +4058,27 @@
         <v>12</v>
       </c>
       <c r="H72" s="28">
-        <v>233794.908861206</v>
+        <v>236120.835873248</v>
       </c>
       <c r="I72" s="34">
         <f t="shared" ref="I72:I73" si="0">H72/E72-1</f>
-        <v>0.14417456070279688</v>
+        <v>0.15555747117844709</v>
       </c>
       <c r="J72" s="35">
-        <f>14.58/1000</f>
-        <v>1.4579999999999999E-2</v>
+        <f>8.25/1000</f>
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="K72" s="1">
-        <f>200 * 10</f>
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="L72" s="24">
         <f t="shared" ref="L72:L73" si="1">K72*J72</f>
-        <v>29.16</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="32">
@@ -4095,11 +4097,11 @@
         <v>47</v>
       </c>
       <c r="H73" s="27">
-        <v>544705.99201381905</v>
+        <v>541477.71245182003</v>
       </c>
       <c r="I73" s="34">
         <f t="shared" si="0"/>
-        <v>0.14269829072051721</v>
+        <v>0.13592592252271962</v>
       </c>
       <c r="J73" s="35">
         <f>44.21/1000</f>

</xml_diff>

<commit_message>
update ALNS parameter values
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5322A317-BEC3-4BF3-B92D-CBE8270542E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F06298-7D8A-42B6-A191-5811FAFB037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="48309" windowHeight="26546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,15 +71,6 @@
     <t>                    :swap!</t>
   </si>
   <si>
-    <t>        σ₁  =   33                      ,</t>
-  </si>
-  <si>
-    <t>        σ₂  =   9                       ,</t>
-  </si>
-  <si>
-    <t>        σ₃  =   13                      ,</t>
-  </si>
-  <si>
     <t>        ω   =   0.05                    ,</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>        𝜃   =   0.99975                 ,</t>
   </si>
   <si>
-    <t>        C̲   =   30                      ,</t>
-  </si>
-  <si>
     <t>        C̅   =   60                      ,</t>
   </si>
   <si>
@@ -318,6 +306,18 @@
   </si>
   <si>
     <t>n = max(500, ceil(x, digits=-(length(digits(x))-1)))</t>
+  </si>
+  <si>
+    <t>        σ₁  =   15                      ,</t>
+  </si>
+  <si>
+    <t>        σ₂  =   10                      ,</t>
+  </si>
+  <si>
+    <t>        σ₃  =   3                       ,</t>
+  </si>
+  <si>
+    <t>        C̲   =   4                       ,</t>
   </si>
 </sst>
 </file>
@@ -944,7 +944,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A50" sqref="A50:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -962,7 +962,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.05" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -980,16 +980,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -997,11 +997,11 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1009,35 +1009,35 @@
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1057,40 +1057,40 @@
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
     </row>
     <row r="18" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8"/>
       <c r="L18" s="12"/>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="19" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B19" s="11"/>
       <c r="L19" s="12"/>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="21" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="22" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="23" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="24" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="25" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="27" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="28" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="29" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="30" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="31" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="32" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="33" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="34" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="35" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="38" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="39" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="40" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="41" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="43" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="44" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="45" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="46" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="47" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="50" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="51" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="52" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="53" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="54" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="55" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="56" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="57" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="58" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="59" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="60" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="61" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B63" s="7"/>
     </row>
@@ -1835,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C64" s="18" t="s">
         <v>0</v>
@@ -1850,7 +1850,7 @@
         <v>4</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H64" s="18" t="s">
         <v>5</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B65" s="2">
         <v>100</v>
@@ -1867,27 +1867,27 @@
         <v>1645.79</v>
       </c>
       <c r="D65" s="6">
-        <v>1643.0888648786899</v>
+        <v>1648.98876590539</v>
       </c>
       <c r="E65" s="3">
         <f>D65/C65-1</f>
-        <v>-1.6412392354492322E-3</v>
+        <v>1.9436051412331512E-3</v>
       </c>
       <c r="F65" s="5">
-        <f>4.84/1000</f>
-        <v>4.8399999999999997E-3</v>
+        <f>4.27/1000</f>
+        <v>4.2699999999999995E-3</v>
       </c>
       <c r="G65" s="1">
         <v>2000</v>
       </c>
       <c r="H65" s="6">
         <f>F65 * G65</f>
-        <v>9.68</v>
+        <v>8.5399999999999991</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B66" s="2">
         <v>100</v>
@@ -1896,27 +1896,27 @@
         <v>1252.3699999999999</v>
       </c>
       <c r="D66" s="24">
-        <v>1196.2386137594799</v>
+        <v>1191.9670339746301</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" ref="E66:E70" si="0">D66/C66-1</f>
-        <v>-4.4820130025886917E-2</v>
+        <v>-4.8230926982736566E-2</v>
       </c>
       <c r="F66" s="4">
-        <f>12.52/1000</f>
-        <v>1.252E-2</v>
+        <f>11.13/1000</f>
+        <v>1.1130000000000001E-2</v>
       </c>
       <c r="G66" s="1">
         <v>2000</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ref="H66:H70" si="1">F66 * G66</f>
-        <v>25.04</v>
+        <v>22.26</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B67" s="2">
         <v>100</v>
@@ -1925,27 +1925,27 @@
         <v>828.94</v>
       </c>
       <c r="D67" s="6">
-        <v>828.93686694224698</v>
+        <v>828.93686694236601</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" si="0"/>
-        <v>-3.7795953302666163E-6</v>
+        <v>-3.7795951867147792E-6</v>
       </c>
       <c r="F67" s="4">
-        <f>6.69/1000</f>
-        <v>6.6900000000000006E-3</v>
+        <f>5.61/1000</f>
+        <v>5.6100000000000004E-3</v>
       </c>
       <c r="G67" s="1">
         <v>2000</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="1"/>
-        <v>13.38</v>
+        <v>11.22</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B68" s="2">
         <v>100</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B69" s="2">
         <v>100</v>
@@ -1983,27 +1983,27 @@
         <v>1696.94</v>
       </c>
       <c r="D69" s="6">
-        <v>1670.2230616634599</v>
+        <v>1669.34791567869</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="0"/>
-        <v>-1.57441856144237E-2</v>
+        <v>-1.6259905666264007E-2</v>
       </c>
       <c r="F69" s="4">
-        <f>5.33/1000</f>
-        <v>5.3299999999999997E-3</v>
+        <f>4.58/1000</f>
+        <v>4.5799999999999999E-3</v>
       </c>
       <c r="G69" s="1">
         <v>2000</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" si="1"/>
-        <v>10.66</v>
+        <v>9.16</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B70" s="2">
         <v>100</v>
@@ -2012,22 +2012,22 @@
         <v>1406.91</v>
       </c>
       <c r="D70" s="24">
-        <v>1297.91070367663</v>
+        <v>1295.0013013222199</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="0"/>
-        <v>-7.7474249471089163E-2</v>
+        <v>-7.9542187259867503E-2</v>
       </c>
       <c r="F70" s="4">
-        <f>12.36/1000</f>
-        <v>1.2359999999999999E-2</v>
+        <f>8.29/1000</f>
+        <v>8.2899999999999988E-3</v>
       </c>
       <c r="G70" s="1">
         <v>2000</v>
       </c>
       <c r="H70" s="6">
         <f t="shared" si="1"/>
-        <v>24.72</v>
+        <v>16.579999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
   <dimension ref="A1:X280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="A53" sqref="A53:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2693,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.05" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -2715,16 +2715,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2734,11 +2734,11 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2748,25 +2748,25 @@
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2776,11 +2776,11 @@
     </row>
     <row r="10" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="12" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2812,11 +2812,11 @@
     </row>
     <row r="13" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2826,11 +2826,11 @@
     </row>
     <row r="14" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2840,11 +2840,11 @@
     </row>
     <row r="15" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -2854,10 +2854,10 @@
     </row>
     <row r="16" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="18" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8"/>
       <c r="L18" s="12"/>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="19" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B19" s="11"/>
       <c r="L19" s="12"/>
@@ -2897,7 +2897,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="21" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="22" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -2948,7 +2948,7 @@
     </row>
     <row r="23" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="24" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="25" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="27" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="28" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="29" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="30" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="31" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="32" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="33" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="34" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="35" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="36" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="37" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="38" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="41" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="42" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="43" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -3389,7 +3389,7 @@
     </row>
     <row r="44" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="46" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="47" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="48" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="49" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="50" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -3578,7 +3578,7 @@
     </row>
     <row r="53" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="54" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="55" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -3638,7 +3638,7 @@
     </row>
     <row r="56" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="57" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="58" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="59" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="60" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="61" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="62" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="63" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="64" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="66" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B66" s="7"/>
       <c r="L66" s="12"/>
@@ -3840,7 +3840,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>0</v>
@@ -3859,7 +3859,7 @@
         <v>4</v>
       </c>
       <c r="K67" s="18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L67" s="18" t="s">
         <v>5</v>
@@ -3876,22 +3876,22 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G68" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H68" s="25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L68" s="12"/>
       <c r="M68" s="12"/>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="69" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="32">
@@ -3924,22 +3924,22 @@
         <v>5</v>
       </c>
       <c r="H69" s="27">
-        <v>55449.609618147799</v>
+        <v>55034.228168332796</v>
       </c>
       <c r="I69" s="34">
         <f>H69/E69-1</f>
-        <v>1.1983458072158726E-2</v>
+        <v>4.4025362424542358E-3</v>
       </c>
       <c r="J69" s="1">
-        <f>0.36/1000</f>
-        <v>3.5999999999999997E-4</v>
+        <f>0.35/1000</f>
+        <v>3.5E-4</v>
       </c>
       <c r="K69" s="1">
         <v>5000</v>
       </c>
       <c r="L69" s="24">
         <f>K69*J69</f>
-        <v>1.7999999999999998</v>
+        <v>1.75</v>
       </c>
       <c r="M69" s="12"/>
       <c r="N69" s="12"/>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="70" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="33">
@@ -3971,22 +3971,22 @@
         <v>6</v>
       </c>
       <c r="H70" s="28">
-        <v>64516.734565587001</v>
+        <v>66423.384898165401</v>
       </c>
       <c r="I70" s="34">
         <f>H70/E70-1</f>
-        <v>2.0156455608409063E-2</v>
+        <v>5.0304938144989153E-2</v>
       </c>
       <c r="J70" s="35">
-        <f>1.5/1000</f>
-        <v>1.5E-3</v>
+        <f>1.37/1000</f>
+        <v>1.3700000000000001E-3</v>
       </c>
       <c r="K70" s="1">
         <v>5000</v>
       </c>
       <c r="L70" s="24">
         <f>K70*J70</f>
-        <v>7.5</v>
+        <v>6.8500000000000005</v>
       </c>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -3999,7 +3999,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="33">
@@ -4018,15 +4018,15 @@
         <v>24</v>
       </c>
       <c r="H71" s="28">
-        <v>207301.86896955999</v>
+        <v>204630.99665072499</v>
       </c>
       <c r="I71" s="34">
         <f>H71/E71-1</f>
-        <v>5.9998920935735889E-2</v>
+        <v>4.6341920205376086E-2</v>
       </c>
       <c r="J71" s="1">
-        <f>5.86/1000</f>
-        <v>5.8600000000000006E-3</v>
+        <f>5.32/1000</f>
+        <v>5.3200000000000001E-3</v>
       </c>
       <c r="K71" s="1">
         <f>200 * 10</f>
@@ -4034,12 +4034,12 @@
       </c>
       <c r="L71" s="24">
         <f>K71*J71</f>
-        <v>11.72</v>
+        <v>10.64</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="33">
@@ -4058,27 +4058,27 @@
         <v>12</v>
       </c>
       <c r="H72" s="28">
-        <v>236120.835873248</v>
+        <v>227835.96029704899</v>
       </c>
       <c r="I72" s="34">
         <f t="shared" ref="I72:I73" si="0">H72/E72-1</f>
-        <v>0.15555747117844709</v>
+        <v>0.11501191815914558</v>
       </c>
       <c r="J72" s="35">
-        <f>8.25/1000</f>
-        <v>8.2500000000000004E-3</v>
+        <f>7.22/1000</f>
+        <v>7.2199999999999999E-3</v>
       </c>
       <c r="K72" s="1">
         <v>5000</v>
       </c>
       <c r="L72" s="24">
         <f t="shared" ref="L72:L73" si="1">K72*J72</f>
-        <v>41.25</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="32">
@@ -4097,22 +4097,22 @@
         <v>47</v>
       </c>
       <c r="H73" s="27">
-        <v>541477.71245182003</v>
+        <v>537694.95265082305</v>
       </c>
       <c r="I73" s="34">
         <f t="shared" si="0"/>
-        <v>0.13592592252271962</v>
+        <v>0.12799035136657211</v>
       </c>
       <c r="J73" s="35">
-        <f>44.21/1000</f>
-        <v>4.4209999999999999E-2</v>
+        <f>28.65/1000</f>
+        <v>2.8649999999999998E-2</v>
       </c>
       <c r="K73" s="1">
         <v>3000</v>
       </c>
       <c r="L73" s="24">
         <f t="shared" si="1"/>
-        <v>132.63</v>
+        <v>85.949999999999989</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update initialization and operations
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F06298-7D8A-42B6-A191-5811FAFB037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A81E7B1-81AD-4B4C-AC63-91B7FBA72F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="48309" windowHeight="26546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VRPTW Benchmarking" sheetId="1" r:id="rId1"/>
@@ -943,24 +943,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X280"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:A60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.05" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>74</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" ht="15.05" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21"/>
@@ -978,12 +978,12 @@
       <c r="E2" s="21"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -995,7 +995,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
@@ -1015,13 +1015,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1041,13 +1041,13 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>39</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -1093,10 +1093,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1115,7 @@
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
@@ -1150,7 +1150,7 @@
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>52</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>53</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>54</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>55</v>
       </c>
@@ -1218,7 +1218,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1235,7 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>56</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
     </row>
-    <row r="29" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>58</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="W29" s="12"/>
       <c r="X29" s="12"/>
     </row>
-    <row r="30" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>59</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="W30" s="12"/>
       <c r="X30" s="12"/>
     </row>
-    <row r="31" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>60</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="W31" s="12"/>
       <c r="X31" s="12"/>
     </row>
-    <row r="32" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>61</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="W32" s="12"/>
       <c r="X32" s="12"/>
     </row>
-    <row r="33" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>62</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="W33" s="12"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>63</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="W34" s="12"/>
       <c r="X34" s="12"/>
     </row>
-    <row r="35" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>64</v>
       </c>
@@ -1388,7 +1388,7 @@
       <c r="W35" s="12"/>
       <c r="X35" s="12"/>
     </row>
-    <row r="36" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>6</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="W36" s="12"/>
       <c r="X36" s="12"/>
     </row>
-    <row r="37" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>9</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
     </row>
-    <row r="38" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>65</v>
       </c>
@@ -1439,7 +1439,7 @@
       <c r="W38" s="12"/>
       <c r="X38" s="12"/>
     </row>
-    <row r="39" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>66</v>
       </c>
@@ -1456,7 +1456,7 @@
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
     </row>
-    <row r="40" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>67</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
     </row>
-    <row r="41" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>68</v>
       </c>
@@ -1490,7 +1490,7 @@
       <c r="W41" s="12"/>
       <c r="X41" s="12"/>
     </row>
-    <row r="42" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1507,7 @@
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
     </row>
-    <row r="43" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>17</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
     </row>
-    <row r="44" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>18</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="W44" s="12"/>
       <c r="X44" s="12"/>
     </row>
-    <row r="45" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>69</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="W45" s="12"/>
       <c r="X45" s="12"/>
     </row>
-    <row r="46" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>70</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="W46" s="12"/>
       <c r="X46" s="12"/>
     </row>
-    <row r="47" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>71</v>
       </c>
@@ -1592,7 +1592,7 @@
       <c r="W47" s="12"/>
       <c r="X47" s="12"/>
     </row>
-    <row r="48" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="W48" s="12"/>
       <c r="X48" s="12"/>
     </row>
-    <row r="49" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +1626,7 @@
       <c r="W49" s="12"/>
       <c r="X49" s="12"/>
     </row>
-    <row r="50" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>90</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="W50" s="12"/>
       <c r="X50" s="12"/>
     </row>
-    <row r="51" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>91</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="W51" s="12"/>
       <c r="X51" s="12"/>
     </row>
-    <row r="52" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>92</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="W52" s="12"/>
       <c r="X52" s="12"/>
     </row>
-    <row r="53" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>11</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
     </row>
-    <row r="54" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>12</v>
       </c>
@@ -1711,7 +1711,7 @@
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
     </row>
-    <row r="55" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>13</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
     </row>
-    <row r="56" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>93</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="W56" s="12"/>
       <c r="X56" s="12"/>
     </row>
-    <row r="57" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>14</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="W57" s="12"/>
       <c r="X57" s="12"/>
     </row>
-    <row r="58" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>15</v>
       </c>
@@ -1779,7 +1779,7 @@
       <c r="W58" s="12"/>
       <c r="X58" s="12"/>
     </row>
-    <row r="59" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>16</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="W59" s="12"/>
       <c r="X59" s="12"/>
     </row>
-    <row r="60" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>72</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="U60" s="12"/>
       <c r="V60" s="12"/>
     </row>
-    <row r="61" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>50</v>
       </c>
@@ -1824,13 +1824,13 @@
       <c r="U61" s="12"/>
       <c r="V61" s="12"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>2</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>44</v>
       </c>
@@ -1867,25 +1867,25 @@
         <v>1645.79</v>
       </c>
       <c r="D65" s="6">
-        <v>1648.98876590539</v>
+        <v>1648.5486688763999</v>
       </c>
       <c r="E65" s="3">
         <f>D65/C65-1</f>
-        <v>1.9436051412331512E-3</v>
+        <v>1.6761973741485914E-3</v>
       </c>
       <c r="F65" s="5">
-        <f>4.27/1000</f>
-        <v>4.2699999999999995E-3</v>
+        <f>4.05/1000</f>
+        <v>4.0499999999999998E-3</v>
       </c>
       <c r="G65" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H65" s="6">
         <f>F65 * G65</f>
-        <v>8.5399999999999991</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
@@ -1896,25 +1896,25 @@
         <v>1252.3699999999999</v>
       </c>
       <c r="D66" s="24">
-        <v>1191.9670339746301</v>
+        <v>1200.2202193455701</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" ref="E66:E70" si="0">D66/C66-1</f>
-        <v>-4.8230926982736566E-2</v>
+        <v>-4.1640873427525316E-2</v>
       </c>
       <c r="F66" s="4">
-        <f>11.13/1000</f>
-        <v>1.1130000000000001E-2</v>
+        <f>10.75/1000</f>
+        <v>1.0749999999999999E-2</v>
       </c>
       <c r="G66" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ref="H66:H70" si="1">F66 * G66</f>
-        <v>22.26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53.749999999999993</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>46</v>
       </c>
@@ -1932,18 +1932,18 @@
         <v>-3.7795951867147792E-6</v>
       </c>
       <c r="F67" s="4">
-        <f>5.61/1000</f>
-        <v>5.6100000000000004E-3</v>
+        <f>5.3/1000</f>
+        <v>5.3E-3</v>
       </c>
       <c r="G67" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="1"/>
-        <v>11.22</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>47</v>
       </c>
@@ -1961,18 +1961,18 @@
         <v>-5.8207641997487514E-6</v>
       </c>
       <c r="F68" s="4">
-        <f>22.87/1000</f>
-        <v>2.2870000000000001E-2</v>
+        <f>17.59/1000</f>
+        <v>1.7590000000000001E-2</v>
       </c>
       <c r="G68" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H68" s="6">
         <f t="shared" si="1"/>
-        <v>45.74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87.95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>48</v>
       </c>
@@ -1983,25 +1983,25 @@
         <v>1696.94</v>
       </c>
       <c r="D69" s="6">
-        <v>1669.34791567869</v>
+        <v>1663.9923050791599</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="0"/>
-        <v>-1.6259905666264007E-2</v>
+        <v>-1.941594571454508E-2</v>
       </c>
       <c r="F69" s="4">
-        <f>4.58/1000</f>
-        <v>4.5799999999999999E-3</v>
+        <f>4.42/1000</f>
+        <v>4.4200000000000003E-3</v>
       </c>
       <c r="G69" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" si="1"/>
-        <v>9.16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>49</v>
       </c>
@@ -2012,652 +2012,652 @@
         <v>1406.91</v>
       </c>
       <c r="D70" s="24">
-        <v>1295.0013013222199</v>
+        <v>1305.8353114469801</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="0"/>
-        <v>-7.9542187259867503E-2</v>
+        <v>-7.1841616416842613E-2</v>
       </c>
       <c r="F70" s="4">
-        <f>8.29/1000</f>
-        <v>8.2899999999999988E-3</v>
+        <f>8.81/1000</f>
+        <v>8.8100000000000001E-3</v>
       </c>
       <c r="G70" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H70" s="6">
         <f t="shared" si="1"/>
-        <v>16.579999999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>44.05</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B72" s="7"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="7"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="7"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="7"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="7"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="7"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="7"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="7"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="7"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="7"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="7"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="7"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="7"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="7"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="7"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="7"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="7"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="7"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="7"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="7"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="7"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="7"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="7"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="7"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="7"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="7"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="7"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="7"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="7"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="7"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="7"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="7"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="7"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="7"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="7"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" s="7"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="7"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="7"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="7"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" s="7"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" s="7"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="7"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="7"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="7"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="7"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="7"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="7"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="7"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" s="7"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="7"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="7"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="7"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="7"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="7"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="7"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="7"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="7"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="7"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="7"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="7"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="7"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="7"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="7"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="7"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="7"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" s="7"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" s="7"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" s="7"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" s="7"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" s="7"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" s="7"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" s="7"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B169" s="7"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" s="7"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" s="7"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" s="7"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" s="7"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B174" s="7"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B175" s="7"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" s="7"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="7"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="7"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="7"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="7"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="7"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="7"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="7"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="7"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="7"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="7"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="7"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="7"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="7"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="7"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="7"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="7"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="7"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="7"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="7"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="7"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="7"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="7"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="7"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="7"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="7"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" s="7"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" s="7"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" s="7"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" s="7"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" s="7"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" s="7"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" s="7"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="7"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="7"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="7"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="7"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="7"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="7"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="7"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="7"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="7"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="7"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="7"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="7"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="7"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="7"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="7"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="7"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" s="7"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" s="7"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" s="7"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" s="7"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" s="7"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" s="7"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" s="7"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" s="7"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B233" s="7"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B234" s="7"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" s="7"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" s="7"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" s="7"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="7"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" s="7"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" s="7"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="7"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="7"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="7"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="7"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="7"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="7"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="7"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="7"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="7"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="7"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="7"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="7"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="7"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="7"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="7"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="7"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" s="7"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" s="7"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" s="7"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" s="7"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B261" s="7"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B262" s="7"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B263" s="7"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B264" s="7"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B265" s="7"/>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B266" s="7"/>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B267" s="7"/>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B268" s="7"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B269" s="7"/>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B270" s="7"/>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B271" s="7"/>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B272" s="7"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" s="7"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" s="7"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" s="7"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="7"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" s="7"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" s="7"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" s="7"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="7"/>
     </row>
   </sheetData>
@@ -2670,28 +2670,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5551421D-4FE7-47B7-A546-15E7A05240A9}">
   <dimension ref="A1:X280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:A63"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.05" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>75</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="15.05" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21"/>
@@ -2713,12 +2713,12 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
@@ -2754,13 +2754,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2798,7 +2798,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>39</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2838,7 +2838,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2852,7 +2852,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -2864,10 +2864,10 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -2886,7 +2886,7 @@
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
@@ -2895,7 +2895,7 @@
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>89</v>
       </c>
@@ -2904,7 +2904,7 @@
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
@@ -2925,7 +2925,7 @@
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>52</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>53</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>54</v>
       </c>
@@ -2988,7 +2988,7 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>55</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>8</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>56</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
@@ -3072,7 +3072,7 @@
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
     </row>
-    <row r="29" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>58</v>
       </c>
@@ -3093,7 +3093,7 @@
       <c r="W29" s="12"/>
       <c r="X29" s="12"/>
     </row>
-    <row r="30" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>76</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="W30" s="12"/>
       <c r="X30" s="12"/>
     </row>
-    <row r="31" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>59</v>
       </c>
@@ -3135,7 +3135,7 @@
       <c r="W31" s="12"/>
       <c r="X31" s="12"/>
     </row>
-    <row r="32" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>60</v>
       </c>
@@ -3156,7 +3156,7 @@
       <c r="W32" s="12"/>
       <c r="X32" s="12"/>
     </row>
-    <row r="33" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>61</v>
       </c>
@@ -3177,7 +3177,7 @@
       <c r="W33" s="12"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>77</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="W34" s="12"/>
       <c r="X34" s="12"/>
     </row>
-    <row r="35" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>62</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="W35" s="12"/>
       <c r="X35" s="12"/>
     </row>
-    <row r="36" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>63</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="W36" s="12"/>
       <c r="X36" s="12"/>
     </row>
-    <row r="37" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>78</v>
       </c>
@@ -3261,7 +3261,7 @@
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
     </row>
-    <row r="38" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>79</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="W38" s="12"/>
       <c r="X38" s="12"/>
     </row>
-    <row r="39" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>6</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
     </row>
-    <row r="40" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>9</v>
       </c>
@@ -3324,7 +3324,7 @@
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
     </row>
-    <row r="41" spans="1:24" s="9" customFormat="1" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>65</v>
       </c>
@@ -3345,7 +3345,7 @@
       <c r="W41" s="12"/>
       <c r="X41" s="12"/>
     </row>
-    <row r="42" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>66</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
     </row>
-    <row r="43" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>67</v>
       </c>
@@ -3387,7 +3387,7 @@
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
     </row>
-    <row r="44" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>68</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="W44" s="12"/>
       <c r="X44" s="12"/>
     </row>
-    <row r="45" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>7</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="W45" s="12"/>
       <c r="X45" s="12"/>
     </row>
-    <row r="46" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>17</v>
       </c>
@@ -3450,7 +3450,7 @@
       <c r="W46" s="12"/>
       <c r="X46" s="12"/>
     </row>
-    <row r="47" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>18</v>
       </c>
@@ -3471,7 +3471,7 @@
       <c r="W47" s="12"/>
       <c r="X47" s="12"/>
     </row>
-    <row r="48" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>69</v>
       </c>
@@ -3492,7 +3492,7 @@
       <c r="W48" s="12"/>
       <c r="X48" s="12"/>
     </row>
-    <row r="49" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>70</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="W49" s="12"/>
       <c r="X49" s="12"/>
     </row>
-    <row r="50" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>71</v>
       </c>
@@ -3534,7 +3534,7 @@
       <c r="W50" s="12"/>
       <c r="X50" s="12"/>
     </row>
-    <row r="51" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>10</v>
       </c>
@@ -3555,7 +3555,7 @@
       <c r="W51" s="12"/>
       <c r="X51" s="12"/>
     </row>
-    <row r="52" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>7</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="W52" s="12"/>
       <c r="X52" s="12"/>
     </row>
-    <row r="53" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>90</v>
       </c>
@@ -3597,7 +3597,7 @@
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
     </row>
-    <row r="54" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>91</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
     </row>
-    <row r="55" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>92</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
     </row>
-    <row r="56" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>11</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="W56" s="12"/>
       <c r="X56" s="12"/>
     </row>
-    <row r="57" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>12</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="W57" s="12"/>
       <c r="X57" s="12"/>
     </row>
-    <row r="58" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>13</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="W58" s="12"/>
       <c r="X58" s="12"/>
     </row>
-    <row r="59" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>93</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="W59" s="12"/>
       <c r="X59" s="12"/>
     </row>
-    <row r="60" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>14</v>
       </c>
@@ -3739,7 +3739,7 @@
       <c r="U60" s="12"/>
       <c r="V60" s="12"/>
     </row>
-    <row r="61" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>15</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="U61" s="12"/>
       <c r="V61" s="12"/>
     </row>
-    <row r="62" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>16</v>
       </c>
@@ -3775,7 +3775,7 @@
       <c r="S62" s="12"/>
       <c r="T62" s="12"/>
     </row>
-    <row r="63" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>72</v>
       </c>
@@ -3792,7 +3792,7 @@
       <c r="S63" s="12"/>
       <c r="T63" s="12"/>
     </row>
-    <row r="64" spans="1:24" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>50</v>
       </c>
@@ -3809,7 +3809,7 @@
       <c r="S64" s="12"/>
       <c r="T64" s="12"/>
     </row>
-    <row r="65" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
       <c r="N65" s="12"/>
@@ -3820,7 +3820,7 @@
       <c r="S65" s="12"/>
       <c r="T65" s="12"/>
     </row>
-    <row r="66" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>22</v>
       </c>
@@ -3835,7 +3835,7 @@
       <c r="S66" s="12"/>
       <c r="T66" s="12"/>
     </row>
-    <row r="67" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>2</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="S67" s="12"/>
       <c r="T67" s="12"/>
     </row>
-    <row r="68" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="25" t="s">
@@ -3903,7 +3903,7 @@
       <c r="S68" s="12"/>
       <c r="T68" s="12"/>
     </row>
-    <row r="69" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>83</v>
       </c>
@@ -3924,22 +3924,22 @@
         <v>5</v>
       </c>
       <c r="H69" s="27">
-        <v>55034.228168332796</v>
+        <v>55089.753137909604</v>
       </c>
       <c r="I69" s="34">
         <f>H69/E69-1</f>
-        <v>4.4025362424542358E-3</v>
+        <v>5.4158950579381582E-3</v>
       </c>
       <c r="J69" s="1">
-        <f>0.35/1000</f>
-        <v>3.5E-4</v>
+        <f>0.32/1000</f>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="K69" s="1">
         <v>5000</v>
       </c>
       <c r="L69" s="24">
         <f>K69*J69</f>
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="M69" s="12"/>
       <c r="N69" s="12"/>
@@ -3950,7 +3950,7 @@
       <c r="S69" s="12"/>
       <c r="T69" s="12"/>
     </row>
-    <row r="70" spans="1:20" ht="15.05" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3971,22 +3971,22 @@
         <v>6</v>
       </c>
       <c r="H70" s="28">
-        <v>66423.384898165401</v>
+        <v>63215.202234419397</v>
       </c>
       <c r="I70" s="34">
         <f>H70/E70-1</f>
-        <v>5.0304938144989153E-2</v>
+        <v>-4.2373368300496761E-4</v>
       </c>
       <c r="J70" s="35">
-        <f>1.37/1000</f>
-        <v>1.3700000000000001E-3</v>
+        <f>1.32/1000</f>
+        <v>1.32E-3</v>
       </c>
       <c r="K70" s="1">
         <v>5000</v>
       </c>
       <c r="L70" s="24">
         <f>K70*J70</f>
-        <v>6.8500000000000005</v>
+        <v>6.6</v>
       </c>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -3997,7 +3997,7 @@
       <c r="S70" s="12"/>
       <c r="T70" s="12"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -4018,15 +4018,15 @@
         <v>24</v>
       </c>
       <c r="H71" s="28">
-        <v>204630.99665072499</v>
+        <v>215209.433732365</v>
       </c>
       <c r="I71" s="34">
         <f>H71/E71-1</f>
-        <v>4.6341920205376086E-2</v>
+        <v>0.10043275859222867</v>
       </c>
       <c r="J71" s="1">
-        <f>5.32/1000</f>
-        <v>5.3200000000000001E-3</v>
+        <f>3.82/1000</f>
+        <v>3.82E-3</v>
       </c>
       <c r="K71" s="1">
         <f>200 * 10</f>
@@ -4034,10 +4034,10 @@
       </c>
       <c r="L71" s="24">
         <f>K71*J71</f>
-        <v>10.64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+        <v>7.64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -4058,25 +4058,25 @@
         <v>12</v>
       </c>
       <c r="H72" s="28">
-        <v>227835.96029704899</v>
+        <v>224500.96823680701</v>
       </c>
       <c r="I72" s="34">
         <f t="shared" ref="I72:I73" si="0">H72/E72-1</f>
-        <v>0.11501191815914558</v>
+        <v>9.8690719831683316E-2</v>
       </c>
       <c r="J72" s="35">
-        <f>7.22/1000</f>
-        <v>7.2199999999999999E-3</v>
+        <f>5.79/1000</f>
+        <v>5.79E-3</v>
       </c>
       <c r="K72" s="1">
         <v>5000</v>
       </c>
       <c r="L72" s="24">
         <f t="shared" ref="L72:L73" si="1">K72*J72</f>
-        <v>36.1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+        <v>28.95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>86</v>
       </c>
@@ -4097,643 +4097,643 @@
         <v>47</v>
       </c>
       <c r="H73" s="27">
-        <v>537694.95265082305</v>
+        <v>513966.62484081602</v>
       </c>
       <c r="I73" s="34">
         <f t="shared" si="0"/>
-        <v>0.12799035136657211</v>
+        <v>7.821245277965283E-2</v>
       </c>
       <c r="J73" s="35">
-        <f>28.65/1000</f>
-        <v>2.8649999999999998E-2</v>
+        <f>16.59/1000</f>
+        <v>1.6590000000000001E-2</v>
       </c>
       <c r="K73" s="1">
         <v>3000</v>
       </c>
       <c r="L73" s="24">
         <f t="shared" si="1"/>
-        <v>85.949999999999989</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+        <v>49.77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="7"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="7"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="7"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="7"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="7"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="7"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="7"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="7"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="7"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="7"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="7"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="7"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="7"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="7"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="7"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="7"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="7"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="7"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="7"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="7"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="7"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="7"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="7"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="7"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="7"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="7"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="7"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="7"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="7"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="7"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="7"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="7"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="7"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="7"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" s="7"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="7"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="7"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="7"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" s="7"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" s="7"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="7"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="7"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="7"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="7"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="7"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="7"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="7"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" s="7"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="7"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="7"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="7"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="7"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="7"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="7"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="7"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="7"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="7"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="7"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="7"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="7"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="7"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="7"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="7"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="7"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" s="7"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" s="7"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" s="7"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" s="7"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" s="7"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" s="7"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" s="7"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B169" s="7"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" s="7"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" s="7"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" s="7"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" s="7"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B174" s="7"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B175" s="7"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" s="7"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="7"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="7"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="7"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="7"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="7"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="7"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="7"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="7"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="7"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="7"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="7"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="7"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="7"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="7"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="7"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="7"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="7"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="7"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="7"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="7"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="7"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="7"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="7"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="7"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="7"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" s="7"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" s="7"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" s="7"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" s="7"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" s="7"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" s="7"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" s="7"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="7"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="7"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="7"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="7"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="7"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="7"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="7"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="7"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="7"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="7"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="7"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="7"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="7"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="7"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="7"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="7"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" s="7"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" s="7"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" s="7"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" s="7"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" s="7"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" s="7"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" s="7"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" s="7"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B233" s="7"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B234" s="7"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" s="7"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" s="7"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" s="7"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="7"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" s="7"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" s="7"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="7"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="7"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="7"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="7"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="7"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="7"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="7"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="7"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="7"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="7"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="7"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="7"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="7"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="7"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="7"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="7"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" s="7"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" s="7"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" s="7"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" s="7"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B261" s="7"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B262" s="7"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B263" s="7"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B264" s="7"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B265" s="7"/>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B266" s="7"/>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B267" s="7"/>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B268" s="7"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B269" s="7"/>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B270" s="7"/>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B271" s="7"/>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B272" s="7"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" s="7"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" s="7"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" s="7"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="7"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" s="7"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" s="7"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" s="7"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more LRP instances
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A81E7B1-81AD-4B4C-AC63-91B7FBA72F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F23746-A83D-4DE3-A52E-D58E5C349C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VRPTW Benchmarking" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="99">
   <si>
     <t>Best known</t>
   </si>
@@ -287,21 +287,6 @@
     <t>Total cost</t>
   </si>
   <si>
-    <t>coord20-5-1</t>
-  </si>
-  <si>
-    <t>coord50-5-1b</t>
-  </si>
-  <si>
-    <t>coord100-5-2</t>
-  </si>
-  <si>
-    <t>coord200-10-3</t>
-  </si>
-  <si>
-    <t>coord100-10-2b</t>
-  </si>
-  <si>
     <t>n = max(200, ceil(x, digits=-(length(digits(x))-1)))</t>
   </si>
   <si>
@@ -318,6 +303,36 @@
   </si>
   <si>
     <t>        C̲   =   4                       ,</t>
+  </si>
+  <si>
+    <t>prins20-5-1</t>
+  </si>
+  <si>
+    <t>prins50-5-1b</t>
+  </si>
+  <si>
+    <t>prins100-5-2</t>
+  </si>
+  <si>
+    <t>prins100-10-2b</t>
+  </si>
+  <si>
+    <t>gaskell36-5</t>
+  </si>
+  <si>
+    <t>daskin88-8</t>
+  </si>
+  <si>
+    <t>christofides100-10</t>
+  </si>
+  <si>
+    <t>min134-8</t>
+  </si>
+  <si>
+    <t>prins200-10-3</t>
+  </si>
+  <si>
+    <t>daskin150-10</t>
   </si>
 </sst>
 </file>
@@ -943,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -1126,7 +1141,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -1628,7 +1643,7 @@
     </row>
     <row r="50" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -1645,7 +1660,7 @@
     </row>
     <row r="51" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -1662,7 +1677,7 @@
     </row>
     <row r="52" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -1730,7 +1745,7 @@
     </row>
     <row r="56" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -2668,10 +2683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5551421D-4FE7-47B7-A546-15E7A05240A9}">
-  <dimension ref="A1:X280"/>
+  <dimension ref="A1:X285"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2897,7 +2912,7 @@
     </row>
     <row r="20" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" s="11"/>
       <c r="L20" s="12"/>
@@ -3578,7 +3593,7 @@
     </row>
     <row r="53" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -3599,7 +3614,7 @@
     </row>
     <row r="54" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -3617,7 +3632,7 @@
     </row>
     <row r="55" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -3701,7 +3716,7 @@
     </row>
     <row r="59" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -3905,7 +3920,7 @@
     </row>
     <row r="69" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="32">
@@ -3952,41 +3967,41 @@
     </row>
     <row r="70" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D70" s="33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E70" s="30">
-        <v>63242</v>
+        <v>460.4</v>
       </c>
       <c r="F70" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" s="33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H70" s="28">
-        <v>63215.202234419397</v>
+        <v>470.215268434927</v>
       </c>
       <c r="I70" s="34">
         <f>H70/E70-1</f>
-        <v>-4.2373368300496761E-4</v>
+        <v>2.1319001813481897E-2</v>
       </c>
       <c r="J70" s="35">
-        <f>1.32/1000</f>
-        <v>1.32E-3</v>
+        <f>0.6/1000</f>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="K70" s="1">
         <v>5000</v>
       </c>
       <c r="L70" s="24">
         <f>K70*J70</f>
-        <v>6.6</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -3997,138 +4012,333 @@
       <c r="S70" s="12"/>
       <c r="T70" s="12"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="33">
         <v>2</v>
       </c>
       <c r="D71" s="33">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E71" s="30">
-        <v>195568</v>
+        <v>63242</v>
       </c>
       <c r="F71" s="33">
         <v>2</v>
       </c>
       <c r="G71" s="33">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H71" s="28">
-        <v>215209.433732365</v>
+        <v>63215.202234419397</v>
       </c>
       <c r="I71" s="34">
         <f>H71/E71-1</f>
+        <v>-4.2373368300496761E-4</v>
+      </c>
+      <c r="J71" s="35">
+        <f>1.32/1000</f>
+        <v>1.32E-3</v>
+      </c>
+      <c r="K71" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L71" s="24">
+        <f>K71*J71</f>
+        <v>6.6</v>
+      </c>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12"/>
+      <c r="T71" s="12"/>
+    </row>
+    <row r="72" spans="1:20" ht="14" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="33">
+        <v>2</v>
+      </c>
+      <c r="D72" s="33">
+        <v>7</v>
+      </c>
+      <c r="E72" s="30">
+        <v>355.8</v>
+      </c>
+      <c r="F72" s="33">
+        <v>2</v>
+      </c>
+      <c r="G72" s="33">
+        <v>7</v>
+      </c>
+      <c r="H72" s="28">
+        <v>356.02826243842702</v>
+      </c>
+      <c r="I72" s="34">
+        <f>H72/E72-1</f>
+        <v>6.4154704448293742E-4</v>
+      </c>
+      <c r="J72" s="35">
+        <f>4.36/1000</f>
+        <v>4.3600000000000002E-3</v>
+      </c>
+      <c r="K72" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L72" s="24">
+        <f t="shared" ref="L72:L78" si="0">K72*J72</f>
+        <v>21.8</v>
+      </c>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="12"/>
+      <c r="S72" s="12"/>
+      <c r="T72" s="12"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="33">
+        <v>2</v>
+      </c>
+      <c r="D73" s="33">
+        <v>24</v>
+      </c>
+      <c r="E73" s="30">
+        <v>195568</v>
+      </c>
+      <c r="F73" s="33">
+        <v>2</v>
+      </c>
+      <c r="G73" s="33">
+        <v>24</v>
+      </c>
+      <c r="H73" s="28">
+        <v>215209.433732365</v>
+      </c>
+      <c r="I73" s="34">
+        <f>H73/E73-1</f>
         <v>0.10043275859222867</v>
       </c>
-      <c r="J71" s="1">
+      <c r="J73" s="1">
         <f>3.82/1000</f>
         <v>3.82E-3</v>
       </c>
-      <c r="K71" s="1">
-        <f>200 * 10</f>
-        <v>2000</v>
-      </c>
-      <c r="L71" s="24">
-        <f>K71*J71</f>
-        <v>7.64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="33">
+      <c r="K73" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L73" s="24">
+        <f t="shared" si="0"/>
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="33">
         <v>3</v>
       </c>
-      <c r="D72" s="33">
+      <c r="D74" s="33">
         <v>11</v>
       </c>
-      <c r="E72" s="30">
+      <c r="E74" s="30">
         <v>204335</v>
       </c>
-      <c r="F72" s="33">
+      <c r="F74" s="33">
         <v>3</v>
       </c>
-      <c r="G72" s="33">
+      <c r="G74" s="33">
         <v>12</v>
       </c>
-      <c r="H72" s="28">
+      <c r="H74" s="28">
         <v>224500.96823680701</v>
       </c>
-      <c r="I72" s="34">
-        <f t="shared" ref="I72:I73" si="0">H72/E72-1</f>
+      <c r="I74" s="34">
+        <f t="shared" ref="I74:I78" si="1">H74/E74-1</f>
         <v>9.8690719831683316E-2</v>
       </c>
-      <c r="J72" s="35">
+      <c r="J74" s="35">
         <f>5.79/1000</f>
         <v>5.79E-3</v>
       </c>
-      <c r="K72" s="1">
+      <c r="K74" s="1">
         <v>5000</v>
       </c>
-      <c r="L72" s="24">
-        <f t="shared" ref="L72:L73" si="1">K72*J72</f>
+      <c r="L74" s="24">
+        <f t="shared" si="0"/>
         <v>28.95</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="32">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="33">
+        <v>2</v>
+      </c>
+      <c r="D75" s="33">
+        <v>8</v>
+      </c>
+      <c r="E75" s="30">
+        <v>842.9</v>
+      </c>
+      <c r="F75" s="33">
+        <v>2</v>
+      </c>
+      <c r="G75" s="33">
+        <v>8</v>
+      </c>
+      <c r="H75" s="28">
+        <v>849.62218670261404</v>
+      </c>
+      <c r="I75" s="34">
+        <f t="shared" si="1"/>
+        <v>7.9750702368182047E-3</v>
+      </c>
+      <c r="J75" s="35">
+        <f>5.65/1000</f>
+        <v>5.6500000000000005E-3</v>
+      </c>
+      <c r="K75" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L75" s="24">
+        <f t="shared" si="0"/>
+        <v>28.250000000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="33">
         <v>3</v>
       </c>
-      <c r="D73" s="32">
+      <c r="D76" s="33">
+        <v>11</v>
+      </c>
+      <c r="E76" s="30">
+        <v>5809</v>
+      </c>
+      <c r="F76" s="33">
+        <v>4</v>
+      </c>
+      <c r="G76" s="33">
+        <v>10</v>
+      </c>
+      <c r="H76" s="28">
+        <v>6111.3704662733498</v>
+      </c>
+      <c r="I76" s="34">
+        <f t="shared" si="1"/>
+        <v>5.205206856143052E-2</v>
+      </c>
+      <c r="J76" s="35">
+        <f>12.93/1000</f>
+        <v>1.2930000000000001E-2</v>
+      </c>
+      <c r="K76" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L76" s="24">
+        <f t="shared" si="0"/>
+        <v>64.650000000000006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="33">
+        <v>3</v>
+      </c>
+      <c r="D77" s="33">
+        <v>11</v>
+      </c>
+      <c r="E77" s="30">
+        <v>44011.7</v>
+      </c>
+      <c r="F77" s="33">
+        <v>3</v>
+      </c>
+      <c r="G77" s="33">
+        <v>11</v>
+      </c>
+      <c r="H77" s="28">
+        <v>46066.884016841599</v>
+      </c>
+      <c r="I77" s="34">
+        <f t="shared" si="1"/>
+        <v>4.6696310681968667E-2</v>
+      </c>
+      <c r="J77" s="35">
+        <f>17.12/1000</f>
+        <v>1.712E-2</v>
+      </c>
+      <c r="K77" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L77" s="24">
+        <f t="shared" si="0"/>
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="32">
+        <v>3</v>
+      </c>
+      <c r="D78" s="32">
         <v>47</v>
       </c>
-      <c r="E73" s="31">
+      <c r="E78" s="31">
         <v>476684</v>
       </c>
-      <c r="F73" s="32">
+      <c r="F78" s="32">
         <v>3</v>
       </c>
-      <c r="G73" s="32">
+      <c r="G78" s="32">
         <v>47</v>
       </c>
-      <c r="H73" s="27">
+      <c r="H78" s="27">
         <v>513966.62484081602</v>
       </c>
-      <c r="I73" s="34">
-        <f t="shared" si="0"/>
+      <c r="I78" s="34">
+        <f t="shared" si="1"/>
         <v>7.821245277965283E-2</v>
       </c>
-      <c r="J73" s="35">
+      <c r="J78" s="35">
         <f>16.59/1000</f>
         <v>1.6590000000000001E-2</v>
       </c>
-      <c r="K73" s="1">
-        <v>3000</v>
-      </c>
-      <c r="L73" s="24">
-        <f t="shared" si="1"/>
-        <v>49.77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B74" s="7"/>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B75" s="7"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B76" s="7"/>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B77" s="7"/>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B78" s="7"/>
+      <c r="K78" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L78" s="24">
+        <f t="shared" si="0"/>
+        <v>82.95</v>
+      </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
@@ -4735,6 +4945,21 @@
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="7"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="7"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="7"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="7"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="7"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
combine inter intra opt
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research related\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842FED09-A8F6-47F1-9C2F-A8B052EDA56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39F0438-BC01-4BDB-AEC6-5C55F9699B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>Best known</t>
   </si>
@@ -199,12 +199,6 @@
     <t>                    :regret3!</t>
   </si>
   <si>
-    <t>                    :intraopt!      ,</t>
-  </si>
-  <si>
-    <t>                    :interopt!      ,</t>
-  </si>
-  <si>
     <t>                    :split!         ,</t>
   </si>
   <si>
@@ -314,6 +308,9 @@
   </si>
   <si>
     <t>                    :move!          ,</t>
+  </si>
+  <si>
+    <t>                    :opt!           ,</t>
   </si>
 </sst>
 </file>
@@ -936,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5551421D-4FE7-47B7-A546-15E7A05240A9}">
-  <dimension ref="A1:X288"/>
+  <dimension ref="A1:X287"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -961,7 +958,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15"/>
@@ -1112,7 +1109,7 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -1125,7 +1122,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -1156,7 +1153,7 @@
     </row>
     <row r="19" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" s="10"/>
       <c r="L19" s="11"/>
@@ -1165,7 +1162,7 @@
     </row>
     <row r="20" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="10"/>
       <c r="L20" s="11"/>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="21" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1363,7 +1360,7 @@
     </row>
     <row r="30" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1447,7 +1444,7 @@
     </row>
     <row r="34" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="37" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1531,7 +1528,7 @@
     </row>
     <row r="38" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1594,7 +1591,7 @@
     </row>
     <row r="41" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -1615,7 +1612,7 @@
     </row>
     <row r="42" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -1636,7 +1633,7 @@
     </row>
     <row r="43" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1657,7 +1654,7 @@
     </row>
     <row r="44" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1762,7 +1759,7 @@
     </row>
     <row r="49" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -1783,7 +1780,7 @@
     </row>
     <row r="50" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -1804,7 +1801,7 @@
     </row>
     <row r="51" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -1825,7 +1822,7 @@
     </row>
     <row r="52" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -1846,7 +1843,7 @@
     </row>
     <row r="53" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -1867,7 +1864,7 @@
     </row>
     <row r="54" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -1888,7 +1885,7 @@
     </row>
     <row r="55" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="56" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -1918,9 +1915,6 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
       <c r="S56" s="11"/>
       <c r="T56" s="11"/>
       <c r="U56" s="11"/>
@@ -1930,7 +1924,7 @@
     </row>
     <row r="57" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -1939,6 +1933,9 @@
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="4"/>
+      <c r="Q57" s="5"/>
       <c r="S57" s="11"/>
       <c r="T57" s="11"/>
       <c r="U57" s="11"/>
@@ -1948,7 +1945,7 @@
     </row>
     <row r="58" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -1957,9 +1954,9 @@
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="4"/>
-      <c r="Q58" s="5"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
@@ -1969,7 +1966,7 @@
     </row>
     <row r="59" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -1990,7 +1987,7 @@
     </row>
     <row r="60" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -2011,7 +2008,7 @@
     </row>
     <row r="61" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -2032,7 +2029,7 @@
     </row>
     <row r="62" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -2048,12 +2045,10 @@
       <c r="T62" s="11"/>
       <c r="U62" s="11"/>
       <c r="V62" s="11"/>
-      <c r="W62" s="11"/>
-      <c r="X62" s="11"/>
     </row>
     <row r="63" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -2072,7 +2067,7 @@
     </row>
     <row r="64" spans="1:24" ht="14" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -2086,12 +2081,10 @@
       <c r="R64" s="11"/>
       <c r="S64" s="11"/>
       <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="11"/>
     </row>
     <row r="65" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -2108,7 +2101,7 @@
     </row>
     <row r="66" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -2124,16 +2117,10 @@
       <c r="T66" s="11"/>
     </row>
     <row r="67" spans="1:20" ht="14" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
       <c r="P67" s="11"/>
       <c r="Q67" s="11"/>
       <c r="R67" s="11"/>
@@ -2141,6 +2128,10 @@
       <c r="T67" s="11"/>
     </row>
     <row r="68" spans="1:20" ht="14" x14ac:dyDescent="0.3">
+      <c r="A68" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="6"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
       <c r="N68" s="11"/>
@@ -2152,12 +2143,34 @@
       <c r="T68" s="11"/>
     </row>
     <row r="69" spans="1:20" ht="14" x14ac:dyDescent="0.3">
-      <c r="A69" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="6"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
+      <c r="A69" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J69" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L69" s="17" t="s">
+        <v>5</v>
+      </c>
       <c r="N69" s="11"/>
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
@@ -2167,34 +2180,28 @@
       <c r="T69" s="11"/>
     </row>
     <row r="70" spans="1:20" ht="14" x14ac:dyDescent="0.3">
-      <c r="A70" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K70" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L70" s="17" t="s">
-        <v>5</v>
-      </c>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F70" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H70" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
       <c r="N70" s="11"/>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -2204,27 +2211,43 @@
       <c r="T70" s="11"/>
     </row>
     <row r="71" spans="1:20" ht="14" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
+      <c r="A71" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D71" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="F71" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G71" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="L71" s="11"/>
+      <c r="C71" s="31">
+        <v>3</v>
+      </c>
+      <c r="D71" s="31">
+        <v>5</v>
+      </c>
+      <c r="E71" s="29">
+        <v>54793</v>
+      </c>
+      <c r="F71" s="31">
+        <v>3</v>
+      </c>
+      <c r="G71" s="31">
+        <v>5</v>
+      </c>
+      <c r="H71" s="26">
+        <v>54778.441645771403</v>
+      </c>
+      <c r="I71" s="33">
+        <f>H71/E71-1</f>
+        <v>-2.6569733777304094E-4</v>
+      </c>
+      <c r="J71" s="1">
+        <f>0.34/1000</f>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="K71" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L71" s="23">
+        <f>K71*J71</f>
+        <v>1.7000000000000002</v>
+      </c>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11"/>
@@ -2235,42 +2258,42 @@
       <c r="T71" s="11"/>
     </row>
     <row r="72" spans="1:20" ht="14" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>70</v>
+      <c r="A72" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="31">
-        <v>3</v>
-      </c>
-      <c r="D72" s="31">
-        <v>5</v>
+      <c r="C72" s="32">
+        <v>1</v>
+      </c>
+      <c r="D72" s="32">
+        <v>4</v>
       </c>
       <c r="E72" s="29">
-        <v>54793</v>
-      </c>
-      <c r="F72" s="31">
-        <v>3</v>
-      </c>
-      <c r="G72" s="31">
-        <v>5</v>
-      </c>
-      <c r="H72" s="26">
-        <v>54778.441645771403</v>
+        <v>460.4</v>
+      </c>
+      <c r="F72" s="32">
+        <v>1</v>
+      </c>
+      <c r="G72" s="32">
+        <v>4</v>
+      </c>
+      <c r="H72" s="27">
+        <v>460.37420333966799</v>
       </c>
       <c r="I72" s="33">
         <f>H72/E72-1</f>
-        <v>-2.6569733777304094E-4</v>
-      </c>
-      <c r="J72" s="1">
-        <f>0.33/1000</f>
-        <v>3.3E-4</v>
+        <v>-5.6030973788034899E-5</v>
+      </c>
+      <c r="J72" s="34">
+        <f>0.6/1000</f>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="K72" s="1">
         <v>5000</v>
       </c>
       <c r="L72" s="23">
         <f>K72*J72</f>
-        <v>1.65</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
@@ -2283,41 +2306,41 @@
     </row>
     <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" s="32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E73" s="29">
-        <v>460.4</v>
+        <v>63242</v>
       </c>
       <c r="F73" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G73" s="32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H73" s="27">
-        <v>460.37420333966799</v>
+        <v>63274.563449802801</v>
       </c>
       <c r="I73" s="33">
         <f>H73/E73-1</f>
-        <v>-5.6030973788034899E-5</v>
+        <v>5.1490227701211921E-4</v>
       </c>
       <c r="J73" s="34">
-        <f>0.67/1000</f>
-        <v>6.7000000000000002E-4</v>
+        <f>1.47/1000</f>
+        <v>1.47E-3</v>
       </c>
       <c r="K73" s="1">
         <v>5000</v>
       </c>
       <c r="L73" s="23">
         <f>K73*J73</f>
-        <v>3.35</v>
+        <v>7.35</v>
       </c>
       <c r="M73" s="11"/>
       <c r="N73" s="11"/>
@@ -2330,41 +2353,41 @@
     </row>
     <row r="74" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="32">
         <v>2</v>
       </c>
       <c r="D74" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E74" s="29">
-        <v>63242</v>
+        <v>355.8</v>
       </c>
       <c r="F74" s="32">
         <v>2</v>
       </c>
       <c r="G74" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H74" s="27">
-        <v>63274.563449802801</v>
+        <v>356.77719975659801</v>
       </c>
       <c r="I74" s="33">
         <f>H74/E74-1</f>
-        <v>5.1490227701211921E-4</v>
+        <v>2.7464861062338475E-3</v>
       </c>
       <c r="J74" s="34">
-        <f>1.53/1000</f>
-        <v>1.5300000000000001E-3</v>
+        <f>6/1000</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K74" s="1">
         <v>5000</v>
       </c>
       <c r="L74" s="23">
-        <f>K74*J74</f>
-        <v>7.65</v>
+        <f t="shared" ref="L74:L80" si="0">K74*J74</f>
+        <v>30</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -2375,168 +2398,160 @@
       <c r="S74" s="11"/>
       <c r="T74" s="11"/>
     </row>
-    <row r="75" spans="1:20" ht="14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="32">
         <v>2</v>
       </c>
       <c r="D75" s="32">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E75" s="29">
-        <v>355.8</v>
+        <v>195568</v>
       </c>
       <c r="F75" s="32">
         <v>2</v>
       </c>
       <c r="G75" s="32">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H75" s="27">
-        <v>360.943822920061</v>
+        <v>196478.25017821</v>
       </c>
       <c r="I75" s="33">
         <f>H75/E75-1</f>
-        <v>1.445706273204328E-2</v>
-      </c>
-      <c r="J75" s="34">
-        <f>6/1000</f>
-        <v>6.0000000000000001E-3</v>
+        <v>4.6543922227051393E-3</v>
+      </c>
+      <c r="J75" s="1">
+        <f>4.57/1000</f>
+        <v>4.5700000000000003E-3</v>
       </c>
       <c r="K75" s="1">
         <v>5000</v>
       </c>
       <c r="L75" s="23">
-        <f t="shared" ref="L75:L81" si="0">K75*J75</f>
-        <v>30</v>
-      </c>
-      <c r="M75" s="11"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="11"/>
-      <c r="R75" s="11"/>
-      <c r="S75" s="11"/>
-      <c r="T75" s="11"/>
+        <f t="shared" si="0"/>
+        <v>22.85</v>
+      </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D76" s="32">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E76" s="29">
-        <v>195568</v>
+        <v>204335</v>
       </c>
       <c r="F76" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G76" s="32">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H76" s="27">
-        <v>198076.10176990301</v>
+        <v>205456.00059630099</v>
       </c>
       <c r="I76" s="33">
-        <f>H76/E76-1</f>
-        <v>1.282470429673066E-2</v>
-      </c>
-      <c r="J76" s="1">
-        <f>4.95/1000</f>
-        <v>4.9500000000000004E-3</v>
+        <f t="shared" ref="I76:I80" si="1">H76/E76-1</f>
+        <v>5.486091938732951E-3</v>
+      </c>
+      <c r="J76" s="34">
+        <f>7.49/1000</f>
+        <v>7.4900000000000001E-3</v>
       </c>
       <c r="K76" s="1">
         <v>5000</v>
       </c>
       <c r="L76" s="23">
         <f t="shared" si="0"/>
-        <v>24.750000000000004</v>
+        <v>37.450000000000003</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E77" s="29">
-        <v>204335</v>
+        <v>842.9</v>
       </c>
       <c r="F77" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G77" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H77" s="27">
-        <v>204311.38517527201</v>
+        <v>851.32497842789701</v>
       </c>
       <c r="I77" s="33">
-        <f t="shared" ref="I77:I81" si="1">H77/E77-1</f>
-        <v>-1.1556916205246459E-4</v>
+        <f t="shared" si="1"/>
+        <v>9.9952288858666805E-3</v>
       </c>
       <c r="J77" s="34">
-        <f>7.78/1000</f>
-        <v>7.7800000000000005E-3</v>
+        <f>7.34/1000</f>
+        <v>7.3400000000000002E-3</v>
       </c>
       <c r="K77" s="1">
         <v>5000</v>
       </c>
       <c r="L77" s="23">
         <f t="shared" si="0"/>
-        <v>38.900000000000006</v>
+        <v>36.700000000000003</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78" s="32">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E78" s="29">
-        <v>842.9</v>
+        <v>5809</v>
       </c>
       <c r="F78" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G78" s="32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H78" s="27">
-        <v>863.845014543415</v>
+        <v>5801.1377820530697</v>
       </c>
       <c r="I78" s="33">
         <f t="shared" si="1"/>
-        <v>2.4848753758945241E-2</v>
+        <v>-1.3534546302169659E-3</v>
       </c>
       <c r="J78" s="34">
-        <f>8.47/1000</f>
-        <v>8.4700000000000001E-3</v>
+        <f>16.2/1000</f>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="K78" s="1">
         <v>5000</v>
       </c>
       <c r="L78" s="23">
         <f t="shared" si="0"/>
-        <v>42.35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
@@ -2551,7 +2566,7 @@
         <v>11</v>
       </c>
       <c r="E79" s="29">
-        <v>5809</v>
+        <v>44011.7</v>
       </c>
       <c r="F79" s="32">
         <v>3</v>
@@ -2560,145 +2575,109 @@
         <v>11</v>
       </c>
       <c r="H79" s="27">
-        <v>5712.9930253951197</v>
+        <v>45483.850889982699</v>
       </c>
       <c r="I79" s="33">
         <f t="shared" si="1"/>
-        <v>-1.6527280875345163E-2</v>
+        <v>3.3449080357784489E-2</v>
       </c>
       <c r="J79" s="34">
-        <f>16.91/1000</f>
-        <v>1.6910000000000001E-2</v>
+        <f>24.5/1000</f>
+        <v>2.4500000000000001E-2</v>
       </c>
       <c r="K79" s="1">
         <v>5000</v>
       </c>
       <c r="L79" s="23">
         <f t="shared" si="0"/>
-        <v>84.550000000000011</v>
+        <v>122.5</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>79</v>
+      <c r="A80" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="32">
+      <c r="C80" s="31">
         <v>3</v>
       </c>
-      <c r="D80" s="32">
-        <v>11</v>
-      </c>
-      <c r="E80" s="29">
-        <v>44011.7</v>
-      </c>
-      <c r="F80" s="32">
+      <c r="D80" s="31">
+        <v>47</v>
+      </c>
+      <c r="E80" s="30">
+        <v>476684</v>
+      </c>
+      <c r="F80" s="31">
         <v>3</v>
       </c>
-      <c r="G80" s="32">
-        <v>11</v>
-      </c>
-      <c r="H80" s="27">
-        <v>45193.437758275497</v>
+      <c r="G80" s="31">
+        <v>47</v>
+      </c>
+      <c r="H80" s="26">
+        <v>489155.82084476098</v>
       </c>
       <c r="I80" s="33">
         <f t="shared" si="1"/>
-        <v>2.6850536522686097E-2</v>
+        <v>2.616370770733023E-2</v>
       </c>
       <c r="J80" s="34">
-        <f>24.5/1000</f>
-        <v>2.4500000000000001E-2</v>
+        <f>24.78/1000</f>
+        <v>2.478E-2</v>
       </c>
       <c r="K80" s="1">
         <v>5000</v>
       </c>
       <c r="L80" s="23">
         <f t="shared" si="0"/>
-        <v>122.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="31">
-        <v>3</v>
-      </c>
-      <c r="D81" s="31">
-        <v>47</v>
-      </c>
-      <c r="E81" s="30">
-        <v>476684</v>
-      </c>
-      <c r="F81" s="31">
-        <v>3</v>
-      </c>
-      <c r="G81" s="31">
-        <v>47</v>
-      </c>
-      <c r="H81" s="26">
-        <v>488842.09624820697</v>
-      </c>
-      <c r="I81" s="33">
-        <f t="shared" si="1"/>
-        <v>2.5505568150403501E-2</v>
-      </c>
-      <c r="J81" s="34">
-        <f>22.65/1000</f>
-        <v>2.265E-2</v>
-      </c>
-      <c r="K81" s="1">
-        <v>5000</v>
-      </c>
-      <c r="L81" s="23">
-        <f t="shared" si="0"/>
-        <v>113.25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+        <v>123.9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="6"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="6"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
@@ -3274,13 +3253,10 @@
     <row r="287" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B287" s="6"/>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B288" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="F69:H69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>